<commit_message>
adding dead to code definitions of trapping metadata
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_trapping_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_trapping_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAACB743-EF7E-F44D-8F0C-536868178288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C3A568-039E-8343-9DD8-B1924A001348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37140" yWindow="660" windowWidth="31600" windowHeight="19400" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="179">
   <si>
     <t>first_name</t>
   </si>
@@ -485,9 +485,6 @@
     <t>Whether or not the fish is dead</t>
   </si>
   <si>
-    <t xml:space="preserve">text </t>
-  </si>
-  <si>
     <t>depth</t>
   </si>
   <si>
@@ -570,6 +567,12 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether a fish is dead </t>
   </si>
 </sst>
 </file>
@@ -1166,9 +1169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1295,7 +1298,7 @@
         <v>88</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N4" s="15">
         <v>0.34375</v>
@@ -1315,7 +1318,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>89</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1398,7 +1401,7 @@
         <v>117</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1412,7 +1415,7 @@
         <v>89</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1426,7 +1429,7 @@
         <v>89</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1440,12 +1443,12 @@
         <v>89</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>119</v>
@@ -1454,7 +1457,7 @@
         <v>89</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1477,7 +1480,7 @@
         <v>95</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M14" s="2">
         <v>1</v>
@@ -1497,7 +1500,7 @@
         <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H15" s="16"/>
     </row>
@@ -1512,16 +1515,16 @@
         <v>89</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:14" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>91</v>
@@ -1550,7 +1553,7 @@
         <v>91</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>91</v>
@@ -1565,7 +1568,7 @@
         <v>95</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M18" s="2">
         <v>0</v>
@@ -1576,10 +1579,10 @@
     </row>
     <row r="19" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>89</v>
@@ -1591,10 +1594,10 @@
     </row>
     <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>89</v>
@@ -1605,10 +1608,10 @@
     </row>
     <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>89</v>
@@ -1619,10 +1622,10 @@
     </row>
     <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>91</v>
@@ -1634,7 +1637,7 @@
         <v>91</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>94</v>
@@ -1648,10 +1651,10 @@
     </row>
     <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>89</v>
@@ -1687,9 +1690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1712,7 +1715,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
@@ -1723,7 +1726,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
         <v>102</v>
@@ -1745,7 +1748,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
         <v>101</v>
@@ -1756,7 +1759,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
         <v>123</v>
@@ -1767,7 +1770,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
         <v>124</v>
@@ -1778,7 +1781,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
         <v>125</v>
@@ -1789,7 +1792,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
         <v>126</v>
@@ -1800,7 +1803,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
         <v>128</v>
@@ -1811,7 +1814,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
         <v>127</v>
@@ -1822,7 +1825,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
         <v>103</v>
@@ -1833,7 +1836,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" t="s">
         <v>104</v>
@@ -1844,7 +1847,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
         <v>105</v>
@@ -1855,18 +1858,18 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
         <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B16" t="s">
         <v>129</v>
@@ -1877,7 +1880,7 @@
     </row>
     <row r="17" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
         <v>132</v>
@@ -1888,7 +1891,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s">
         <v>130</v>
@@ -1899,7 +1902,7 @@
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
         <v>131</v>
@@ -1908,8 +1911,16 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="2"/>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>

</xml_diff>

<commit_message>
reordering metadata of trapping
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_trapping_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_trapping_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C3A568-039E-8343-9DD8-B1924A001348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2530B2D-5DA3-434A-8B0F-8919D4E18AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42760" yWindow="1400" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -28,6 +28,14 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -1169,9 +1177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH23"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,175 +1326,205 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>147</v>
+    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>155</v>
+        <v>92</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="14">
-        <v>100000000</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M9" s="2">
         <v>1</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N9" s="14">
         <v>100000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>140</v>
+        <v>92</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="14">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>141</v>
+        <v>92</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>151</v>
+        <v>92</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>142</v>
+    <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2">
-        <v>1</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1519,62 +1557,32 @@
       </c>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="1:14" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>149</v>
+    <row r="17" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0</v>
-      </c>
-      <c r="N17" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>91</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>151</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2">
-        <v>1000</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1665,18 +1673,18 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D14 D1:D10 D25:D1026 D16:D23" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31:D1032 D18:D23 D1:D23 D19:D23" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:F1026 F1:F23" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F31:F1032 F18:F23 F19:F23 F1:F23" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I14 I16:I1026" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I23 I30:I1032" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G14 G16:G1026" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G23 G30:G1032" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1690,9 +1698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>